<commit_message>
Updated xls file with user distribution graphs
</commit_message>
<xml_diff>
--- a/topic_modeling/twitter/Run1-Distributions.xlsx
+++ b/topic_modeling/twitter/Run1-Distributions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="1680" windowWidth="28720" windowHeight="16320" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,19 +24,62 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>0.0.00158881185934</t>
+  </si>
+  <si>
+    <t>Commercial Growers</t>
+  </si>
+  <si>
+    <t>Non-Profits</t>
+  </si>
+  <si>
+    <t>Service Providers</t>
+  </si>
+  <si>
+    <t>News</t>
+  </si>
+  <si>
+    <t>Interest Groups</t>
+  </si>
+  <si>
+    <t>Shops</t>
+  </si>
+  <si>
+    <t>Individuals</t>
+  </si>
+  <si>
+    <t># of Users</t>
+  </si>
+  <si>
+    <t># of Tweets</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -59,13 +102,45 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="17">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -263,11 +338,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1976490272"/>
-        <c:axId val="-1978316304"/>
+        <c:axId val="-2139284128"/>
+        <c:axId val="-2139277056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1976490272"/>
+        <c:axId val="-2139284128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -324,12 +399,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1978316304"/>
+        <c:crossAx val="-2139277056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1978316304"/>
+        <c:axId val="-2139277056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -386,7 +461,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1976490272"/>
+        <c:crossAx val="-2139284128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -620,11 +695,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2036614640"/>
-        <c:axId val="-1978917376"/>
+        <c:axId val="-2139712704"/>
+        <c:axId val="-2139706528"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2036614640"/>
+        <c:axId val="-2139712704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -681,12 +756,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1978917376"/>
+        <c:crossAx val="-2139706528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1978917376"/>
+        <c:axId val="-2139706528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -743,7 +818,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2036614640"/>
+        <c:crossAx val="-2139712704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -977,11 +1052,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2096010384"/>
-        <c:axId val="-1976698624"/>
+        <c:axId val="-2139724112"/>
+        <c:axId val="-2139804816"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2096010384"/>
+        <c:axId val="-2139724112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1038,12 +1113,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1976698624"/>
+        <c:crossAx val="-2139804816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1976698624"/>
+        <c:axId val="-2139804816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1100,7 +1175,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2096010384"/>
+        <c:crossAx val="-2139724112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1334,11 +1409,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2006864976"/>
-        <c:axId val="-2008104608"/>
+        <c:axId val="-2090550000"/>
+        <c:axId val="-2090543792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2006864976"/>
+        <c:axId val="-2090550000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1395,12 +1470,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2008104608"/>
+        <c:crossAx val="-2090543792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2008104608"/>
+        <c:axId val="-2090543792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1457,7 +1532,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2006864976"/>
+        <c:crossAx val="-2090550000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1691,11 +1766,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1973892144"/>
-        <c:axId val="-1973861568"/>
+        <c:axId val="-2090515904"/>
+        <c:axId val="-2090509696"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1973892144"/>
+        <c:axId val="-2090515904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1752,12 +1827,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1973861568"/>
+        <c:crossAx val="-2090509696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1973861568"/>
+        <c:axId val="-2090509696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1814,7 +1889,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1973892144"/>
+        <c:crossAx val="-2090515904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2048,11 +2123,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2006084880"/>
-        <c:axId val="-1973259984"/>
+        <c:axId val="-2090484912"/>
+        <c:axId val="-2090478720"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2006084880"/>
+        <c:axId val="-2090484912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2109,12 +2184,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1973259984"/>
+        <c:crossAx val="-2090478720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1973259984"/>
+        <c:axId val="-2090478720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2171,7 +2246,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2006084880"/>
+        <c:crossAx val="-2090484912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2405,11 +2480,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1978909840"/>
-        <c:axId val="-1979675632"/>
+        <c:axId val="-2090454144"/>
+        <c:axId val="-2090447936"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1978909840"/>
+        <c:axId val="-2090454144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2466,12 +2541,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1979675632"/>
+        <c:crossAx val="-2090447936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1979675632"/>
+        <c:axId val="-2090447936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2528,7 +2603,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1978909840"/>
+        <c:crossAx val="-2090454144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2553,6 +2628,1144 @@
         <a:schemeClr val="tx1">
           <a:lumMod val="15000"/>
           <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$L$50</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v># of Users</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.0547095166474977"/>
+                  <c:y val="0.0127747642655779"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.441719455011944"/>
+                  <c:y val="-0.0884811898512686"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.30074272317084"/>
+                  <c:y val="0.0047994556236026"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.399496888731605"/>
+                  <c:y val="0.0602399144551375"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.237259282196467"/>
+                  <c:y val="0.10981841158744"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.0719549382169924"/>
+                  <c:y val="0.0852114319043453"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:pattFill prst="pct75">
+                <a:fgClr>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="50000"/>
+                      <a:lumOff val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$M$49:$S$49</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Non-Profits</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Commercial Growers</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>News</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Service Providers</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Interest Groups</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Shops</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Individuals</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$M$50:$S$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>84.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>114.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2322.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="1"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.747468961042791"/>
+          <c:y val="0.61215942451638"/>
+          <c:w val="0.230059128844849"/>
+          <c:h val="0.326236609312725"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="39000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+        <a:gs pos="39000">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="lt1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="25000"/>
+          <a:lumOff val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$L$50</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v># of Users</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.0547095166474977"/>
+                  <c:y val="0.0127747642655779"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.441719455011944"/>
+                  <c:y val="-0.0884811898512686"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.30074272317084"/>
+                  <c:y val="0.0047994556236026"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.399496888731605"/>
+                  <c:y val="0.0602399144551375"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.237259282196467"/>
+                  <c:y val="0.10981841158744"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.0719549382169924"/>
+                  <c:y val="0.0852114319043453"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:pattFill prst="pct75">
+                <a:fgClr>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="50000"/>
+                      <a:lumOff val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$M$49:$S$49</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Non-Profits</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Commercial Growers</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>News</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Service Providers</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Interest Groups</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Shops</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Individuals</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$M$50:$S$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>84.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>114.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2322.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="1"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.747468961042791"/>
+          <c:y val="0.61215942451638"/>
+          <c:w val="0.230059128844849"/>
+          <c:h val="0.326236609312725"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="39000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+        <a:gs pos="39000">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="lt1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="25000"/>
+          <a:lumOff val="75000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:round/>
@@ -2857,6 +4070,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -6465,6 +7758,1208 @@
         <a:noFill/>
       </a:ln>
     </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="253">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="all" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="39000">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="pct75">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="pct75">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+                <a:alpha val="42000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="36000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+                <a:alpha val="42000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="36000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+          <a:alpha val="39000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="253">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="all" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="39000">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="pct75">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="pct75">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+                <a:alpha val="42000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="36000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+                <a:alpha val="42000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="36000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+          <a:alpha val="39000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -6681,6 +9176,70 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 9"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Chart 10"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6947,10 +9506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L55"/>
+  <dimension ref="A1:S55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="L48" sqref="L48"/>
+    <sheetView tabSelected="1" topLeftCell="C37" workbookViewId="0">
+      <selection activeCell="N50" sqref="N50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7349,31 +9908,100 @@
         <v>4.8324254420100002E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>2</v>
       </c>
       <c r="B49">
         <v>0.96133931833800002</v>
       </c>
+      <c r="M49" t="s">
+        <v>2</v>
+      </c>
+      <c r="N49" t="s">
+        <v>1</v>
+      </c>
+      <c r="O49" t="s">
+        <v>4</v>
+      </c>
+      <c r="P49" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>5</v>
+      </c>
+      <c r="R49" t="s">
+        <v>6</v>
+      </c>
+      <c r="S49" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>3</v>
       </c>
       <c r="B50">
         <v>4.8324579180700003E-3</v>
       </c>
+      <c r="L50" t="s">
+        <v>8</v>
+      </c>
+      <c r="M50">
+        <v>1</v>
+      </c>
+      <c r="N50">
+        <v>7</v>
+      </c>
+      <c r="O50">
+        <v>30</v>
+      </c>
+      <c r="P50">
+        <v>84</v>
+      </c>
+      <c r="Q50">
+        <v>100</v>
+      </c>
+      <c r="R50">
+        <v>114</v>
+      </c>
+      <c r="S50">
+        <v>2322</v>
+      </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>4</v>
       </c>
       <c r="B51">
         <v>4.8326654384699998E-3</v>
       </c>
+      <c r="L51" t="s">
+        <v>9</v>
+      </c>
+      <c r="M51">
+        <v>8</v>
+      </c>
+      <c r="N51">
+        <v>2</v>
+      </c>
+      <c r="O51">
+        <v>149</v>
+      </c>
+      <c r="P51">
+        <v>153</v>
+      </c>
+      <c r="Q51">
+        <v>342</v>
+      </c>
+      <c r="R51">
+        <v>363</v>
+      </c>
+      <c r="S51">
+        <v>3068</v>
+      </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>5</v>
       </c>
@@ -7381,7 +10009,7 @@
         <v>4.8339451502000001E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>6</v>
       </c>
@@ -7389,7 +10017,7 @@
         <v>4.8326574956900001E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>7</v>
       </c>
@@ -7397,7 +10025,7 @@
         <v>4.8322781778800004E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>8</v>
       </c>
@@ -7407,6 +10035,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>